<commit_message>
Actualizacion Tareas Diagrama de Gantt
</commit_message>
<xml_diff>
--- a/Diagrama Gantt Tecnovnetas.xlsx
+++ b/Diagrama Gantt Tecnovnetas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marip\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6152e9a17840b269/Documentos/Tecnoventas-document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C36DFA1-8B1A-48DF-9BBF-87DD37F56701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{3C36DFA1-8B1A-48DF-9BBF-87DD37F56701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D03474FB-9D79-4100-9FD7-1E10F87A720E}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -474,6 +474,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -492,7 +493,6 @@
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -796,8 +796,8 @@
   <dimension ref="A1:AV30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
+      <pane ySplit="6" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -816,10 +816,10 @@
       <c r="A4" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="45"/>
+      <c r="C4" s="46"/>
       <c r="D4" s="30">
         <v>0</v>
       </c>
@@ -827,46 +827,46 @@
         <f>D5+D4</f>
         <v>45078</v>
       </c>
-      <c r="G4" s="47">
+      <c r="G4" s="48">
         <f>G5</f>
         <v>45078</v>
       </c>
-      <c r="H4" s="48"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="48"/>
-      <c r="M4" s="49"/>
-      <c r="N4" s="47">
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="50"/>
+      <c r="N4" s="48">
         <f>N5</f>
         <v>45085</v>
       </c>
-      <c r="O4" s="48"/>
-      <c r="P4" s="48"/>
-      <c r="Q4" s="48"/>
-      <c r="R4" s="48"/>
-      <c r="S4" s="48"/>
-      <c r="T4" s="49"/>
-      <c r="U4" s="47">
+      <c r="O4" s="49"/>
+      <c r="P4" s="49"/>
+      <c r="Q4" s="49"/>
+      <c r="R4" s="49"/>
+      <c r="S4" s="49"/>
+      <c r="T4" s="50"/>
+      <c r="U4" s="48">
         <f>U5</f>
         <v>45092</v>
       </c>
-      <c r="V4" s="48"/>
-      <c r="W4" s="48"/>
-      <c r="X4" s="48"/>
-      <c r="Y4" s="48"/>
-      <c r="Z4" s="48"/>
-      <c r="AA4" s="49"/>
-      <c r="AB4" s="47">
+      <c r="V4" s="49"/>
+      <c r="W4" s="49"/>
+      <c r="X4" s="49"/>
+      <c r="Y4" s="49"/>
+      <c r="Z4" s="49"/>
+      <c r="AA4" s="50"/>
+      <c r="AB4" s="48">
         <f>AB5</f>
         <v>45099</v>
       </c>
-      <c r="AC4" s="48"/>
-      <c r="AD4" s="48"/>
-      <c r="AE4" s="48"/>
-      <c r="AF4" s="48"/>
-      <c r="AG4" s="48"/>
-      <c r="AH4" s="49"/>
+      <c r="AC4" s="49"/>
+      <c r="AD4" s="49"/>
+      <c r="AE4" s="49"/>
+      <c r="AF4" s="49"/>
+      <c r="AG4" s="49"/>
+      <c r="AH4" s="50"/>
       <c r="AI4" s="41"/>
       <c r="AJ4" s="42"/>
       <c r="AK4" s="42"/>
@@ -883,15 +883,15 @@
       <c r="AV4" s="43"/>
     </row>
     <row r="5" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="50">
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="51">
         <v>45078</v>
       </c>
-      <c r="E5" s="50"/>
+      <c r="E5" s="51"/>
       <c r="F5" s="7"/>
       <c r="G5" s="24">
         <f>E4</f>
@@ -1880,7 +1880,7 @@
         <v>14</v>
       </c>
       <c r="C19" s="9">
-        <v>0.65</v>
+        <v>0.9</v>
       </c>
       <c r="D19" s="6">
         <v>45224</v>
@@ -1998,7 +1998,7 @@
         <v>0</v>
       </c>
       <c r="C21" s="9">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="D21" s="6">
         <v>45255</v>
@@ -2291,7 +2291,7 @@
         <v>47</v>
       </c>
       <c r="C29" s="9">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="D29" s="6">
         <v>45323</v>
@@ -2301,7 +2301,7 @@
       </c>
     </row>
     <row r="30" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="C30" s="51"/>
+      <c r="C30" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Actualizacion Diagrama de Gantt
</commit_message>
<xml_diff>
--- a/Diagrama Gantt Tecnovnetas.xlsx
+++ b/Diagrama Gantt Tecnovnetas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6152e9a17840b269/Documentos/Tecnoventas-document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{3C36DFA1-8B1A-48DF-9BBF-87DD37F56701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D03474FB-9D79-4100-9FD7-1E10F87A720E}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{3C36DFA1-8B1A-48DF-9BBF-87DD37F56701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00E991FB-87DB-46E7-8B55-C3920E284360}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
   <si>
     <t>Santiago</t>
   </si>
@@ -139,9 +139,6 @@
     <t>Seleccionar productos a comparar</t>
   </si>
   <si>
-    <t>Santiago, Paula, Diego</t>
-  </si>
-  <si>
     <t>Modificar precio</t>
   </si>
   <si>
@@ -163,7 +160,7 @@
     <t>Boton de Ayuda</t>
   </si>
   <si>
-    <t>Diego, Lisbeth, Sofia</t>
+    <t>Santiago, Paula</t>
   </si>
 </sst>
 </file>
@@ -796,8 +793,8 @@
   <dimension ref="A1:AV30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
+      <pane ySplit="6" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -814,10 +811,10 @@
     </row>
     <row r="4" spans="1:48" ht="14" x14ac:dyDescent="0.3">
       <c r="A4" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="46" t="s">
         <v>44</v>
-      </c>
-      <c r="B4" s="46" t="s">
-        <v>45</v>
       </c>
       <c r="C4" s="46"/>
       <c r="D4" s="30">
@@ -884,7 +881,7 @@
     </row>
     <row r="5" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A5" s="47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" s="47"/>
       <c r="C5" s="47"/>
@@ -1579,7 +1576,7 @@
     </row>
     <row r="14" spans="1:48" s="13" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>1</v>
@@ -1638,10 +1635,10 @@
     </row>
     <row r="15" spans="1:48" s="13" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="15" t="s">
         <v>41</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>42</v>
       </c>
       <c r="C15" s="9">
         <v>1</v>
@@ -2054,10 +2051,10 @@
         <v>6</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C22" s="9">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="D22" s="6">
         <v>45255</v>
@@ -2283,21 +2280,21 @@
       <c r="N28" s="33"/>
       <c r="O28" s="33"/>
     </row>
-    <row r="29" spans="1:48" ht="25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:48" ht="14" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>47</v>
+        <v>3</v>
       </c>
       <c r="C29" s="9">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="D29" s="6">
         <v>45323</v>
       </c>
       <c r="E29" s="6">
-        <v>45352</v>
+        <v>45334</v>
       </c>
     </row>
     <row r="30" spans="1:48" x14ac:dyDescent="0.25">

</xml_diff>